<commit_message>
finished Section 1, adds other section (empty)
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-01.data.xlsx
+++ b/artifact/data/rdbms-01.data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/sentry/sentry-tutorial/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexiality/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="12540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9140" yWindow="-20560" windowWidth="16800" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>true</t>
   </si>
@@ -88,128 +88,199 @@
     <t>false</t>
   </si>
   <si>
-    <t>qapay01.autocommit</t>
-  </si>
-  <si>
-    <t>qapay01.password</t>
-  </si>
-  <si>
-    <t>qapay01.type</t>
-  </si>
-  <si>
     <t>db2</t>
   </si>
   <si>
-    <t>qapay01.url</t>
+    <t>mssql</t>
+  </si>
+  <si>
+    <t>&lt;null&gt;</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>select * from db2.payroll_batch where CLIENT_ID = ${client}</t>
+  </si>
+  <si>
+    <t>39832</t>
+  </si>
+  <si>
+    <t>my baseline</t>
+  </si>
+  <si>
+    <t>$(syspath|data|fullpath)/baseline.csv</t>
+  </si>
+  <si>
+    <t>crypt:... ... ...</t>
+  </si>
+  <si>
+    <r>
+      <t>jdbc:sqlserver://</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>server</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>\</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>schema</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>port</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>;databaseName=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>database_name</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>jdbc:connx:DD=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>datafile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>;GateWay=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>gateway_server</t>
+    </r>
+  </si>
+  <si>
+    <t>my_db2.type</t>
+  </si>
+  <si>
+    <t>my_db2.url</t>
+  </si>
+  <si>
+    <t>my_db2.user</t>
+  </si>
+  <si>
+    <t>my_db2.password</t>
+  </si>
+  <si>
+    <t>my_db2.autocommit</t>
+  </si>
+  <si>
+    <t>my_db2 select1</t>
+  </si>
+  <si>
+    <t>my_sqlserver.type</t>
+  </si>
+  <si>
+    <t>my_sqlserver.url</t>
+  </si>
+  <si>
+    <t>my_sqlserver.user</t>
+  </si>
+  <si>
+    <t>my_sqlserver.password</t>
+  </si>
+  <si>
+    <t>my_sqlserver.autocommit</t>
+  </si>
+  <si>
+    <t>my_sqlserver.treatNullAs</t>
+  </si>
+  <si>
+    <t>my_connx.type</t>
+  </si>
+  <si>
+    <t>my_connx</t>
+  </si>
+  <si>
+    <t>my_connx.url</t>
+  </si>
+  <si>
+    <t>my_connx.user</t>
+  </si>
+  <si>
+    <t>my_connx.password</t>
+  </si>
+  <si>
+    <t>my_connx.autocommit</t>
+  </si>
+  <si>
+    <t>tell time</t>
+  </si>
+  <si>
+    <t>SELECT CURRENT_TIMESTAMP FROM SYSIBM.SYSDUMMY1</t>
   </si>
   <si>
     <t>jdbc:db2://csqDB2b1:60100/QAPAY01</t>
   </si>
   <si>
-    <t>qapay01.user</t>
-  </si>
-  <si>
     <t>mb092953</t>
   </si>
   <si>
-    <t>mssql</t>
-  </si>
-  <si>
-    <t>jdbc:sqlserver://CSQPYSQL101\NGP_DATA:1570;databaseName=EpSyncQA</t>
-  </si>
-  <si>
-    <t>crypt:d56b5be38c28ac7bc0194c6b50d1b011163c9b9dc1afa77e</t>
-  </si>
-  <si>
-    <t>&lt;null&gt;</t>
-  </si>
-  <si>
-    <t>crypt:7424731ee827b60f32a8b58ebb4410e3</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>isam</t>
-  </si>
-  <si>
-    <t>jdbc:connx:DD=qapay01files;GateWay=csqconx01</t>
-  </si>
-  <si>
-    <t>crypt:d62924c290361817edf8af9084d5974d650e7c4a48f41f52</t>
-  </si>
-  <si>
-    <t>crypt:17a0f910057e7f7e583e1b6eff2d16382200ced65bb78eab</t>
-  </si>
-  <si>
-    <t>ngpdb.type</t>
-  </si>
-  <si>
-    <t>ngpdb.url</t>
-  </si>
-  <si>
-    <t>ngpdb.user</t>
-  </si>
-  <si>
-    <t>ngpdb.password</t>
-  </si>
-  <si>
-    <t>ngpdb.autocommit</t>
-  </si>
-  <si>
-    <t>ngpdb.treatNullAs</t>
-  </si>
-  <si>
-    <t>qapay01 select1</t>
-  </si>
-  <si>
-    <t>client</t>
-  </si>
-  <si>
-    <t>ngp select1</t>
-  </si>
-  <si>
-    <t>SELECT
- PAYEECATEGORYID   AS "id",
- PAYEECATEGORYCODE AS "code",
- PAYEECATEGORYDESC AS "display"
-FROM EMP_PAYEECATEGORY</t>
-  </si>
-  <si>
-    <t>isam.type</t>
-  </si>
-  <si>
-    <t>isam.url</t>
-  </si>
-  <si>
-    <t>isam.user</t>
-  </si>
-  <si>
-    <t>isam.password</t>
-  </si>
-  <si>
-    <t>isam.autocommit</t>
-  </si>
-  <si>
-    <t>isam select1</t>
-  </si>
-  <si>
-    <t>select proc_control_no from "0000prtprc" where site = 'ZZZ';</t>
-  </si>
-  <si>
     <t>crypt:36e50d467d265a4f1e22640129b68cff1a3d707f2858e1c9</t>
-  </si>
-  <si>
-    <t>select * from db2.payroll_batch where CLIENT_ID = ${client}</t>
-  </si>
-  <si>
-    <t>39832</t>
-  </si>
-  <si>
-    <t>my baseline</t>
-  </si>
-  <si>
-    <t>$(syspath|data|fullpath)/baseline.csv</t>
   </si>
 </sst>
 </file>
@@ -283,7 +354,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -345,96 +416,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </right>
-      <top style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </top>
-      <bottom style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </top>
-      <bottom style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </right>
-      <top style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color theme="6" tint="0.39994506668294322"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -445,7 +426,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -489,54 +470,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -553,6 +486,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -563,7 +505,35 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1050,14 +1020,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView zoomScale="134" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="34" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="77.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="75.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
@@ -1088,7 +1058,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
@@ -1134,52 +1104,52 @@
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
-      <c r="A8" s="19" t="s">
-        <v>14</v>
+      <c r="A8" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" s="7"/>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703">
-      <c r="A9" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>17</v>
+      <c r="A9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>44</v>
       </c>
       <c r="C9" s="7"/>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
     <row r="10" spans="1:703">
-      <c r="A10" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>19</v>
+      <c r="A10" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="C10" s="7"/>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
     <row r="11" spans="1:703">
-      <c r="A11" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>47</v>
+      <c r="A11" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>46</v>
       </c>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:703">
-      <c r="A12" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="23" t="s">
+      <c r="A12" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="7"/>
@@ -1189,96 +1159,96 @@
         <v>30</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:703">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:703">
-      <c r="A15" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>24</v>
-      </c>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:703">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="15" t="s">
-        <v>22</v>
+      <c r="B16" s="17" t="s">
+        <v>21</v>
       </c>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>23</v>
+      <c r="B18" s="13" t="s">
+        <v>14</v>
       </c>
       <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="14" t="s">
+      <c r="B22" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="7"/>
@@ -1290,22 +1260,30 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="14" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="16" priority="3" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="13" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="15" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="5" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="11" priority="4" stopIfTrue="1">
+  <conditionalFormatting sqref="B1:B7 B13:B1048576">
+    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="12" priority="7">
       <formula>LEN(TRIM(B1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
+      <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1317,168 +1295,156 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC08D69-8887-4444-B785-D23953AF8585}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView zoomScale="132" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="34" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="77.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="8.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="56.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
-      <c r="A1" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>48</v>
+      <c r="A1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>43</v>
       </c>
       <c r="C1" s="7"/>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
-      <c r="A2" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>49</v>
-      </c>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="7"/>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
-    <row r="3" spans="1:703" ht="85">
-      <c r="A3" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>39</v>
-      </c>
+    <row r="3" spans="1:703">
+      <c r="A3" s="12"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="7"/>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
     <row r="4" spans="1:703">
-      <c r="A4" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="25" t="s">
-        <v>46</v>
-      </c>
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="7"/>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="7"/>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="7"/>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="7"/>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
-      <c r="A8" s="24"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="7"/>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="7"/>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
     <row r="10" spans="1:703">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="7"/>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
     <row r="11" spans="1:703">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:703">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:703">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:703">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:703">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:703">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3">
@@ -1488,21 +1454,21 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="9" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1515,9 +1481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEF39D-E984-C449-9030-77DFE4612593}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -1529,150 +1493,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:703">
-      <c r="A1" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>48</v>
+      <c r="A1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>17</v>
       </c>
       <c r="C1" s="7"/>
       <c r="HA1" s="6"/>
       <c r="AAA1" s="6"/>
     </row>
     <row r="2" spans="1:703">
-      <c r="A2" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>49</v>
+      <c r="A2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>18</v>
       </c>
       <c r="C2" s="7"/>
       <c r="HA2" s="6"/>
       <c r="AAA2" s="6"/>
     </row>
     <row r="3" spans="1:703">
-      <c r="A3" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>51</v>
+      <c r="A3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="C3" s="7"/>
       <c r="HA3" s="6"/>
       <c r="AAA3" s="6"/>
     </row>
     <row r="4" spans="1:703">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="7"/>
       <c r="HA4" s="4"/>
       <c r="AAA4" s="5"/>
     </row>
     <row r="5" spans="1:703">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
+      <c r="A5" s="12"/>
+      <c r="B5" s="13"/>
       <c r="C5" s="7"/>
       <c r="HA5" s="4"/>
       <c r="AAA5" s="5"/>
     </row>
     <row r="6" spans="1:703">
-      <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="7"/>
       <c r="HA6" s="4"/>
       <c r="AAA6" s="5"/>
     </row>
     <row r="7" spans="1:703">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
       <c r="C7" s="7"/>
       <c r="HA7" s="4"/>
       <c r="AAA7" s="5"/>
     </row>
     <row r="8" spans="1:703">
-      <c r="A8" s="24"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="7"/>
       <c r="HA8" s="4"/>
       <c r="AAA8" s="5"/>
     </row>
     <row r="9" spans="1:703">
-      <c r="A9" s="24"/>
-      <c r="B9" s="25"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="7"/>
       <c r="HA9" s="4"/>
       <c r="AAA9" s="5"/>
     </row>
     <row r="10" spans="1:703">
-      <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="7"/>
       <c r="HA10" s="4"/>
       <c r="AAA10" s="5"/>
     </row>
     <row r="11" spans="1:703">
-      <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:703">
-      <c r="A12" s="24"/>
-      <c r="B12" s="25"/>
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:703">
-      <c r="A13" s="24"/>
-      <c r="B13" s="25"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:703">
-      <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:703">
-      <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:703">
-      <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="24"/>
-      <c r="B22" s="25"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="25"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3">
@@ -1682,21 +1646,21 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="6" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="5" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="4" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
move to use sqlite as example db
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-01.data.xlsx
+++ b/artifact/data/rdbms-01.data.xlsx
@@ -9,15 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="-20560" windowWidth="16800" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="12540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
     <sheet name="HelloWorld" sheetId="3" r:id="rId2"/>
-    <sheet name="db2_payroll_batch" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -37,7 +36,7 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>true</t>
   </si>
@@ -98,21 +97,6 @@
   </si>
   <si>
     <t>0</t>
-  </si>
-  <si>
-    <t>client</t>
-  </si>
-  <si>
-    <t>select * from db2.payroll_batch where CLIENT_ID = ${client}</t>
-  </si>
-  <si>
-    <t>39832</t>
-  </si>
-  <si>
-    <t>my baseline</t>
-  </si>
-  <si>
-    <t>$(syspath|data|fullpath)/baseline.csv</t>
   </si>
   <si>
     <t>crypt:... ... ...</t>
@@ -229,9 +213,6 @@
     <t>my_db2.autocommit</t>
   </si>
   <si>
-    <t>my_db2 select1</t>
-  </si>
-  <si>
     <t>my_sqlserver.type</t>
   </si>
   <si>
@@ -271,23 +252,91 @@
     <t>tell time</t>
   </si>
   <si>
-    <t>SELECT CURRENT_TIMESTAMP FROM SYSIBM.SYSDUMMY1</t>
-  </si>
-  <si>
-    <t>jdbc:db2://csqDB2b1:60100/QAPAY01</t>
-  </si>
-  <si>
-    <t>mb092953</t>
-  </si>
-  <si>
-    <t>crypt:36e50d467d265a4f1e22640129b68cff1a3d707f2858e1c9</t>
+    <r>
+      <t>jdbc:db2://</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>server</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>port</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="1"/>
+      </rPr>
+      <t>database_name</t>
+    </r>
+  </si>
+  <si>
+    <t>mydb.type</t>
+  </si>
+  <si>
+    <t>sqlite</t>
+  </si>
+  <si>
+    <t>mydb.url</t>
+  </si>
+  <si>
+    <t>jdbc:sqlite:$(syspath|out|fullpath)/chinook.db</t>
+  </si>
+  <si>
+    <t>mydb.user</t>
+  </si>
+  <si>
+    <t>(empty)</t>
+  </si>
+  <si>
+    <t>mydb.password</t>
+  </si>
+  <si>
+    <t>mydb.autocommit</t>
+  </si>
+  <si>
+    <t>SELECT datetime(current_timestamp, 'localtime')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -336,6 +385,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Courier New"/>
       <family val="1"/>
     </font>
@@ -505,7 +561,72 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -559,108 +680,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1018,16 +1037,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AAA24"/>
+  <dimension ref="A1:AAA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A7" zoomScale="108" zoomScaleNormal="384" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="75.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="79.5" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
@@ -1105,7 +1124,7 @@
     </row>
     <row r="8" spans="1:703">
       <c r="A8" s="16" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>12</v>
@@ -1116,10 +1135,10 @@
     </row>
     <row r="9" spans="1:703">
       <c r="A9" s="16" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C9" s="7"/>
       <c r="HA9" s="4"/>
@@ -1127,10 +1146,10 @@
     </row>
     <row r="10" spans="1:703">
       <c r="A10" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>45</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="C10" s="7"/>
       <c r="HA10" s="4"/>
@@ -1138,16 +1157,16 @@
     </row>
     <row r="11" spans="1:703">
       <c r="A11" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>46</v>
+        <v>22</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>16</v>
       </c>
       <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:703">
       <c r="A12" s="16" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>0</v>
@@ -1156,7 +1175,7 @@
     </row>
     <row r="13" spans="1:703">
       <c r="A13" s="12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>13</v>
@@ -1165,34 +1184,34 @@
     </row>
     <row r="14" spans="1:703">
       <c r="A14" s="12" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:703">
       <c r="A15" s="12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:703">
       <c r="A16" s="12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>0</v>
@@ -1201,7 +1220,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>14</v>
@@ -1210,43 +1229,43 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>0</v>
@@ -1254,36 +1273,80 @@
       <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="16" priority="3" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="13" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="15" priority="4" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="12" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="14" priority="5" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B7 B13:B1048576">
-    <cfRule type="expression" dxfId="13" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="7">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="9">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:B11">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="5" priority="2">
+      <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1295,8 +1358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC08D69-8887-4444-B785-D23953AF8585}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1310,10 +1373,10 @@
   <sheetData>
     <row r="1" spans="1:703">
       <c r="A1" s="12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C1" s="7"/>
       <c r="HA1" s="6"/>
@@ -1454,213 +1517,21 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="11" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="10" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="9" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="5">
-      <formula>LEN(TRIM(B1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2DEF39D-E984-C449-9030-77DFE4612593}">
-  <dimension ref="A1:AAA24"/>
-  <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
-  <cols>
-    <col min="1" max="1" width="34" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="77.83203125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:703">
-      <c r="A1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="HA1" s="6"/>
-      <c r="AAA1" s="6"/>
-    </row>
-    <row r="2" spans="1:703">
-      <c r="A2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="HA2" s="6"/>
-      <c r="AAA2" s="6"/>
-    </row>
-    <row r="3" spans="1:703">
-      <c r="A3" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="HA3" s="6"/>
-      <c r="AAA3" s="6"/>
-    </row>
-    <row r="4" spans="1:703">
-      <c r="A4" s="12"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="7"/>
-      <c r="HA4" s="4"/>
-      <c r="AAA4" s="5"/>
-    </row>
-    <row r="5" spans="1:703">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="7"/>
-      <c r="HA5" s="4"/>
-      <c r="AAA5" s="5"/>
-    </row>
-    <row r="6" spans="1:703">
-      <c r="A6" s="12"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="7"/>
-      <c r="HA6" s="4"/>
-      <c r="AAA6" s="5"/>
-    </row>
-    <row r="7" spans="1:703">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="7"/>
-      <c r="HA7" s="4"/>
-      <c r="AAA7" s="5"/>
-    </row>
-    <row r="8" spans="1:703">
-      <c r="A8" s="12"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="7"/>
-      <c r="HA8" s="4"/>
-      <c r="AAA8" s="5"/>
-    </row>
-    <row r="9" spans="1:703">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="7"/>
-      <c r="HA9" s="4"/>
-      <c r="AAA9" s="5"/>
-    </row>
-    <row r="10" spans="1:703">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="7"/>
-      <c r="HA10" s="4"/>
-      <c r="AAA10" s="5"/>
-    </row>
-    <row r="11" spans="1:703">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:703">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:703">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:703">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:703">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:703">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="6" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
-      <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="5" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
-      <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="3" stopIfTrue="1">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="3" priority="4" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added section 2, example 1
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-01.data.xlsx
+++ b/artifact/data/rdbms-01.data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="12540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -329,7 +329,7 @@
     <t>mydb.autocommit</t>
   </si>
   <si>
-    <t>SELECT datetime(current_timestamp, 'localtime')</t>
+    <t>SELECT datetime(current_timestamp, 'localtime') AS RIGHT_NOW</t>
   </si>
 </sst>
 </file>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="108" zoomScaleNormal="384" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="108" zoomScaleNormal="384" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1358,14 +1358,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC08D69-8887-4444-B785-D23953AF8585}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="56.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="73.1640625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
     <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
     <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>

</xml_diff>

<commit_message>
- update links, section titles and common styles - added image artifacts and text for section 3
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-01.data.xlsx
+++ b/artifact/data/rdbms-01.data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10124"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexiality/tutorials/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/sentry/sentry-tutorial/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="12540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
     <sheet name="HelloWorld" sheetId="3" r:id="rId2"/>
+    <sheet name="more_dbs" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
   <si>
     <t>true</t>
   </si>
@@ -331,12 +332,90 @@
   <si>
     <t>SELECT datetime(current_timestamp, 'localtime') AS RIGHT_NOW</t>
   </si>
+  <si>
+    <t>qapay01.type</t>
+  </si>
+  <si>
+    <t>qapay01.url</t>
+  </si>
+  <si>
+    <t>jdbc:db2://csqDB2b1:60100/QAPAY01</t>
+  </si>
+  <si>
+    <t>qapay01.user</t>
+  </si>
+  <si>
+    <t>crypt:a5289c946b758658d415c4f887c1aa5c5aee8db9f85b6657</t>
+  </si>
+  <si>
+    <t>qapay01.password</t>
+  </si>
+  <si>
+    <t>crypt:36e50d467d265a4f1e22640129b68cff1a3d707f2858e1c9</t>
+  </si>
+  <si>
+    <t>qapay01.autocommit</t>
+  </si>
+  <si>
+    <t>ngpdb.type</t>
+  </si>
+  <si>
+    <t>ngpdb.url</t>
+  </si>
+  <si>
+    <t>jdbc:sqlserver://CSQPYSQL101\NGP_DATA:1570;databaseName=EpSyncQA</t>
+  </si>
+  <si>
+    <t>ngpdb.user</t>
+  </si>
+  <si>
+    <t>crypt:7424731ee827b60f32a8b58ebb4410e3</t>
+  </si>
+  <si>
+    <t>ngpdb.password</t>
+  </si>
+  <si>
+    <t>crypt:d56b5be38c28ac7bc0194c6b50d1b011163c9b9dc1afa77e</t>
+  </si>
+  <si>
+    <t>ngpdb.autocommit</t>
+  </si>
+  <si>
+    <t>ngpdb.treatNullAs</t>
+  </si>
+  <si>
+    <t>isam.type</t>
+  </si>
+  <si>
+    <t>isam</t>
+  </si>
+  <si>
+    <t>isam.url</t>
+  </si>
+  <si>
+    <t>jdbc:connx:DD=qapay01files;GateWay=csqconx01</t>
+  </si>
+  <si>
+    <t>isam.user</t>
+  </si>
+  <si>
+    <t>crypt:d62924c290361817edf8af9084d5974d650e7c4a48f41f52</t>
+  </si>
+  <si>
+    <t>isam.password</t>
+  </si>
+  <si>
+    <t>crypt:17a0f910057e7f7e583e1b6eff2d16382200ced65bb78eab</t>
+  </si>
+  <si>
+    <t>isam.autocommit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -394,6 +473,14 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -482,7 +569,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -551,6 +638,8 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -561,7 +650,128 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <u val="none"/>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1039,7 +1249,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="108" zoomScaleNormal="384" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="108" zoomScaleNormal="384" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -1315,37 +1525,37 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="13" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="22" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="21" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="11" priority="7" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B7 B13:B1048576">
-    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="8" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="9" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="9">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="7" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="5" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="14" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1517,25 +1727,264 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="13" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="12" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D134DDB-4F16-B545-B019-B88C436CB58C}">
+  <dimension ref="A1:AAA24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="384" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
+  <cols>
+    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="82" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
+    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:703">
+      <c r="A1" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="HA1" s="6"/>
+      <c r="AAA1" s="6"/>
+    </row>
+    <row r="2" spans="1:703">
+      <c r="A2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="HA2" s="6"/>
+      <c r="AAA2" s="6"/>
+    </row>
+    <row r="3" spans="1:703">
+      <c r="A3" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="HA3" s="6"/>
+      <c r="AAA3" s="6"/>
+    </row>
+    <row r="4" spans="1:703">
+      <c r="A4" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="HA4" s="4"/>
+      <c r="AAA4" s="5"/>
+    </row>
+    <row r="5" spans="1:703">
+      <c r="A5" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="HA5" s="4"/>
+      <c r="AAA5" s="5"/>
+    </row>
+    <row r="6" spans="1:703">
+      <c r="A6" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="HA6" s="4"/>
+      <c r="AAA6" s="5"/>
+    </row>
+    <row r="7" spans="1:703">
+      <c r="A7" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="HA7" s="4"/>
+      <c r="AAA7" s="5"/>
+    </row>
+    <row r="8" spans="1:703">
+      <c r="A8" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="HA8" s="4"/>
+      <c r="AAA8" s="5"/>
+    </row>
+    <row r="9" spans="1:703">
+      <c r="A9" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="HA9" s="4"/>
+      <c r="AAA9" s="5"/>
+    </row>
+    <row r="10" spans="1:703">
+      <c r="A10" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="HA10" s="4"/>
+      <c r="AAA10" s="5"/>
+    </row>
+    <row r="11" spans="1:703">
+      <c r="A11" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:703">
+      <c r="A12" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:703">
+      <c r="A13" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="7"/>
+    </row>
+    <row r="14" spans="1:703">
+      <c r="A14" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="7"/>
+    </row>
+    <row r="15" spans="1:703">
+      <c r="A15" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:703">
+      <c r="A16" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+    </row>
+  </sheetData>
+  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
+  <conditionalFormatting sqref="A17:A1048576">
+    <cfRule type="beginsWith" dxfId="8" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+      <formula>LEFT(A17,LEN("sentry.scope."))="sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="7" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
+      <formula>LEFT(A17,LEN("sentry."))="sentry."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="6" priority="7" stopIfTrue="1">
+      <formula>LEN(TRIM(A17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:B1048576">
+    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
+      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
+    </cfRule>
+    <cfRule type="notContainsBlanks" dxfId="4" priority="9">
+      <formula>LEN(TRIM(B17))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- added images for tutorials - merge 'transaction' and 'update multi-sql' tutorial as one
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-01.data.xlsx
+++ b/artifact/data/rdbms-01.data.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10124"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10206"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/sentry/sentry-tutorial/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexiality/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="12540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
     <sheet name="HelloWorld" sheetId="3" r:id="rId2"/>
-    <sheet name="more_dbs" sheetId="4" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="base">'[1]#system'!$B$2:$B$24</definedName>
@@ -37,7 +36,7 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>true</t>
   </si>
@@ -332,90 +331,12 @@
   <si>
     <t>SELECT datetime(current_timestamp, 'localtime') AS RIGHT_NOW</t>
   </si>
-  <si>
-    <t>qapay01.type</t>
-  </si>
-  <si>
-    <t>qapay01.url</t>
-  </si>
-  <si>
-    <t>jdbc:db2://csqDB2b1:60100/QAPAY01</t>
-  </si>
-  <si>
-    <t>qapay01.user</t>
-  </si>
-  <si>
-    <t>crypt:a5289c946b758658d415c4f887c1aa5c5aee8db9f85b6657</t>
-  </si>
-  <si>
-    <t>qapay01.password</t>
-  </si>
-  <si>
-    <t>crypt:36e50d467d265a4f1e22640129b68cff1a3d707f2858e1c9</t>
-  </si>
-  <si>
-    <t>qapay01.autocommit</t>
-  </si>
-  <si>
-    <t>ngpdb.type</t>
-  </si>
-  <si>
-    <t>ngpdb.url</t>
-  </si>
-  <si>
-    <t>jdbc:sqlserver://CSQPYSQL101\NGP_DATA:1570;databaseName=EpSyncQA</t>
-  </si>
-  <si>
-    <t>ngpdb.user</t>
-  </si>
-  <si>
-    <t>crypt:7424731ee827b60f32a8b58ebb4410e3</t>
-  </si>
-  <si>
-    <t>ngpdb.password</t>
-  </si>
-  <si>
-    <t>crypt:d56b5be38c28ac7bc0194c6b50d1b011163c9b9dc1afa77e</t>
-  </si>
-  <si>
-    <t>ngpdb.autocommit</t>
-  </si>
-  <si>
-    <t>ngpdb.treatNullAs</t>
-  </si>
-  <si>
-    <t>isam.type</t>
-  </si>
-  <si>
-    <t>isam</t>
-  </si>
-  <si>
-    <t>isam.url</t>
-  </si>
-  <si>
-    <t>jdbc:connx:DD=qapay01files;GateWay=csqconx01</t>
-  </si>
-  <si>
-    <t>isam.user</t>
-  </si>
-  <si>
-    <t>crypt:d62924c290361817edf8af9084d5974d650e7c4a48f41f52</t>
-  </si>
-  <si>
-    <t>isam.password</t>
-  </si>
-  <si>
-    <t>crypt:17a0f910057e7f7e583e1b6eff2d16382200ced65bb78eab</t>
-  </si>
-  <si>
-    <t>isam.autocommit</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -473,14 +394,6 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -569,7 +482,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -638,8 +551,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -650,128 +561,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <font>
         <b val="0"/>
@@ -1249,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="108" zoomScaleNormal="384" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="108" zoomScaleNormal="384" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1525,37 +1315,37 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="22" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="13" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="21" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="12" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="7" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="7" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B7 B13:B1048576">
-    <cfRule type="expression" dxfId="19" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="9">
+    <cfRule type="notContainsBlanks" dxfId="9" priority="9">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="17" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="3" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="16" priority="4">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="4">
       <formula>LEN(TRIM(B12))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10:B11">
-    <cfRule type="expression" dxfId="15" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="14" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="5" priority="2">
       <formula>LEN(TRIM(B10))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1727,264 +1517,25 @@
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="beginsWith" dxfId="13" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
+    <cfRule type="beginsWith" dxfId="4" priority="1" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
       <formula>LEFT(A1,LEN("sentry.scope."))="sentry.scope."</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="12" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
+    <cfRule type="beginsWith" dxfId="3" priority="2" stopIfTrue="1" operator="beginsWith" text="sentry.">
       <formula>LEFT(A1,LEN("sentry."))="sentry."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="11" priority="3" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="3" stopIfTrue="1">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="expression" dxfId="10" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
       <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="9" priority="5">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="5">
       <formula>LEN(TRIM(B1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D134DDB-4F16-B545-B019-B88C436CB58C}">
-  <dimension ref="A1:AAA24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="384" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
-  <cols>
-    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="82" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="9" width="27" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="27" width="21.1640625" style="3" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="10.83203125" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:703">
-      <c r="A1" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="HA1" s="6"/>
-      <c r="AAA1" s="6"/>
-    </row>
-    <row r="2" spans="1:703">
-      <c r="A2" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="HA2" s="6"/>
-      <c r="AAA2" s="6"/>
-    </row>
-    <row r="3" spans="1:703">
-      <c r="A3" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="HA3" s="6"/>
-      <c r="AAA3" s="6"/>
-    </row>
-    <row r="4" spans="1:703">
-      <c r="A4" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="HA4" s="4"/>
-      <c r="AAA4" s="5"/>
-    </row>
-    <row r="5" spans="1:703">
-      <c r="A5" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="HA5" s="4"/>
-      <c r="AAA5" s="5"/>
-    </row>
-    <row r="6" spans="1:703">
-      <c r="A6" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="HA6" s="4"/>
-      <c r="AAA6" s="5"/>
-    </row>
-    <row r="7" spans="1:703">
-      <c r="A7" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="HA7" s="4"/>
-      <c r="AAA7" s="5"/>
-    </row>
-    <row r="8" spans="1:703">
-      <c r="A8" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="HA8" s="4"/>
-      <c r="AAA8" s="5"/>
-    </row>
-    <row r="9" spans="1:703">
-      <c r="A9" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="HA9" s="4"/>
-      <c r="AAA9" s="5"/>
-    </row>
-    <row r="10" spans="1:703">
-      <c r="A10" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="HA10" s="4"/>
-      <c r="AAA10" s="5"/>
-    </row>
-    <row r="11" spans="1:703">
-      <c r="A11" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:703">
-      <c r="A12" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:703">
-      <c r="A13" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:703">
-      <c r="A14" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:703">
-      <c r="A15" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:703">
-      <c r="A16" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-    </row>
-  </sheetData>
-  <sheetProtection formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
-  <conditionalFormatting sqref="A17:A1048576">
-    <cfRule type="beginsWith" dxfId="8" priority="5" stopIfTrue="1" operator="beginsWith" text="sentry.scope.">
-      <formula>LEFT(A17,LEN("sentry.scope."))="sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="beginsWith" dxfId="7" priority="6" stopIfTrue="1" operator="beginsWith" text="sentry.">
-      <formula>LEFT(A17,LEN("sentry."))="sentry."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="6" priority="7" stopIfTrue="1">
-      <formula>LEN(TRIM(A17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:B1048576">
-    <cfRule type="expression" dxfId="5" priority="8" stopIfTrue="1">
-      <formula>LEFT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1), 13) = "sentry.scope."</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="9">
-      <formula>LEN(TRIM(B17))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- added updated artifact files - some content update for Nexial Expression
Signed-off-by: Mike Liu <mliu@ep.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-01.data.xlsx
+++ b/artifact/data/rdbms-01.data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexiality/tutorials/artifact/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/ep/sentry/tutorial-workspace/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="40960" windowHeight="12540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="108" zoomScaleNormal="384" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A7" zoomScale="108" zoomScaleNormal="384" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
@@ -1358,7 +1358,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC08D69-8887-4444-B785-D23953AF8585}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
minor updates to test artifacts
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-01.data.xlsx
+++ b/artifact/data/rdbms-01.data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10404"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE507CC1-5611-1B47-B2B3-C226C81613DE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC73C8D-7211-6A41-85BD-68D037E8D8A6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7720" yWindow="500" windowWidth="25580" windowHeight="10280" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1320,9 +1320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC08D69-8887-4444-B785-D23953AF8585}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>

</xml_diff>

<commit_message>
updated web tutorial (COMPLETE)
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/artifact/data/rdbms-01.data.xlsx
+++ b/artifact/data/rdbms-01.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/tutorials/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45D30CE0-B814-1E4E-806C-3531280CF81D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DABD78B-46B4-3F44-B46C-92C71E7292BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="10280" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="51200" windowHeight="15780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -41,11 +41,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1045,7 +1040,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
@@ -1325,7 +1322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FC08D69-8887-4444-B785-D23953AF8585}">
   <dimension ref="A1:AAA24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>